<commit_message>
Updating 2022 and 2023 standard deviations so they are both reported at 30 June for their respective year.
</commit_message>
<xml_diff>
--- a/doc/_static/2022-pmhc-outcome-measure-standard-deviations.xlsx
+++ b/doc/_static/2022-pmhc-outcome-measure-standard-deviations.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennib/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennib/Work/git/PMHC/spec/doc/_static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29991BC4-C38F-244C-BB75-103A490B2ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ED83B45-B916-FA4D-9AA5-0AD96517FDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42340" yWindow="7140" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-pmhc-outcome-measure-stand" sheetId="1" r:id="rId1"/>
+    <sheet name="z1 (1)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Report Z1 Measure standard deviations for National; 15/08/2022</t>
+    <t>Report Z1 Measure standard deviations for National; 30/06/2022</t>
   </si>
   <si>
     <t>CO Type</t>
@@ -49,7 +49,7 @@
     <t>K10+</t>
   </si>
   <si>
-    <t>Generated on 17/02/2023 10:21:38 AEDT</t>
+    <t>Generated on 28/09/2023 12:11:18 AEST</t>
   </si>
 </sst>
 </file>
@@ -920,7 +920,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>6.0897413515989998</v>
+        <v>6.1207381871009998</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>5.8086072196660004</v>
+        <v>5.8760869122460004</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -942,7 +942,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>5.8085834591710004</v>
+        <v>5.7114030448179998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>4.9361790491950002</v>
+        <v>4.9510919988840003</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -964,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>8.7083843908990008</v>
+        <v>8.7174795351449994</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>